<commit_message>
- fix bug - add function Search
</commit_message>
<xml_diff>
--- a/Document/ProductBacklog.xlsx
+++ b/Document/ProductBacklog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="85">
   <si>
     <t>create project</t>
   </si>
@@ -230,39 +230,15 @@
     <t>tu dong xac dinh thoi gian dien ra su kien dua vao thoi gian ranh cua thanh vien</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>layout active account</t>
-  </si>
-  <si>
     <t>Issues</t>
   </si>
   <si>
-    <t>login when active</t>
-  </si>
-  <si>
-    <t>cannot change email</t>
-  </si>
-  <si>
-    <t>check form email</t>
-  </si>
-  <si>
-    <t>error mail but still create account</t>
-  </si>
-  <si>
-    <t>cannot delete multility account</t>
-  </si>
-  <si>
     <t>create proccess</t>
   </si>
   <si>
     <t>edit process</t>
   </si>
   <si>
-    <t>isDelete field not hide</t>
-  </si>
-  <si>
     <t>cannot edit</t>
   </si>
   <si>
@@ -272,42 +248,21 @@
     <t>edit class</t>
   </si>
   <si>
-    <t>isDeleted field not hide</t>
-  </si>
-  <si>
     <t>show class</t>
   </si>
   <si>
-    <t>dupplicate Projects field</t>
-  </si>
-  <si>
     <t>parent container --&gt; parent project</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>abort calendar</t>
   </si>
   <si>
     <t>abort process</t>
   </si>
   <si>
-    <t>email is the same email of deleted account</t>
-  </si>
-  <si>
     <t>failed when email not invalid</t>
   </si>
   <si>
-    <t>add account many times</t>
-  </si>
-  <si>
-    <t>add account inactive</t>
-  </si>
-  <si>
-    <t>no remove</t>
-  </si>
-  <si>
     <t>cannot create workitem when not be member</t>
   </si>
   <si>
@@ -317,20 +272,14 @@
     <t>history</t>
   </si>
   <si>
-    <t>not</t>
-  </si>
-  <si>
     <t>my project</t>
-  </si>
-  <si>
-    <t>not load data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,8 +307,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,8 +353,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -423,12 +392,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -440,18 +418,36 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="B1:E35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,8 +910,8 @@
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -938,9 +934,11 @@
       <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>72</v>
-      </c>
+      <c r="F1" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
@@ -956,21 +954,9 @@
       <c r="E2" s="10">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" t="s">
-        <v>75</v>
-      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="18"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -986,10 +972,7 @@
       <c r="E3" s="10">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
@@ -1005,14 +988,12 @@
       <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="15"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>59</v>
@@ -1024,14 +1005,11 @@
       <c r="E5" s="10">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>60</v>
@@ -1043,14 +1021,11 @@
       <c r="E6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>9</v>
@@ -1062,14 +1037,12 @@
       <c r="E7" s="10">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>0</v>
@@ -1082,13 +1055,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="15"/>
+        <v>77</v>
+      </c>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>88</v>
+      <c r="A9" s="10">
+        <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>2</v>
@@ -1100,16 +1073,16 @@
       <c r="E9" s="10">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>90</v>
+      <c r="F9" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>1</v>
@@ -1121,14 +1094,11 @@
       <c r="E10" s="10">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>3</v>
@@ -1140,19 +1110,15 @@
       <c r="E11" s="10">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>94</v>
-      </c>
+      <c r="F11" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>10</v>
@@ -1164,14 +1130,11 @@
       <c r="E12" s="10">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>62</v>
@@ -1183,11 +1146,11 @@
       <c r="E13" s="10">
         <v>1</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>63</v>
@@ -1200,18 +1163,18 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>64</v>
@@ -1223,14 +1186,11 @@
       <c r="E15" s="10">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>51</v>
@@ -1243,13 +1203,13 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="15"/>
+        <v>83</v>
+      </c>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>5</v>
+      <c r="A17" s="10">
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
@@ -1263,14 +1223,12 @@
       <c r="E17" s="4">
         <v>2</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="G17" s="17"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>9</v>
+      <c r="A18" s="10">
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>55</v>
@@ -1282,14 +1240,11 @@
       <c r="E18" s="4">
         <v>2</v>
       </c>
-      <c r="F18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>10</v>
+      <c r="A19" s="10">
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>54</v>
@@ -1301,14 +1256,11 @@
       <c r="E19" s="4">
         <v>2</v>
       </c>
-      <c r="F19" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="17"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>11</v>
+      <c r="A20" s="10">
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>53</v>
@@ -1320,14 +1272,11 @@
       <c r="E20" s="4">
         <v>2</v>
       </c>
-      <c r="F20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="17"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>27</v>
+      <c r="A21" s="10">
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>52</v>
@@ -1339,14 +1288,11 @@
       <c r="E21" s="4">
         <v>2</v>
       </c>
-      <c r="F21" t="s">
-        <v>99</v>
-      </c>
-      <c r="G21" s="17"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>41</v>
+      <c r="A22" s="10">
+        <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>57</v>
@@ -1358,11 +1304,11 @@
       <c r="E22" s="4">
         <v>2</v>
       </c>
-      <c r="G22" s="17"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>42</v>
+      <c r="A23" s="10">
+        <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>56</v>
@@ -1374,11 +1320,11 @@
       <c r="E23" s="4">
         <v>2</v>
       </c>
-      <c r="G23" s="17"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>44</v>
+      <c r="A24" s="10">
+        <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>66</v>
@@ -1390,11 +1336,11 @@
       <c r="E24" s="4">
         <v>2</v>
       </c>
-      <c r="G24" s="17"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>45</v>
+      <c r="A25" s="10">
+        <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>67</v>
@@ -1406,29 +1352,29 @@
       <c r="E25" s="4">
         <v>2</v>
       </c>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
-        <v>46</v>
-      </c>
-      <c r="B26" s="13" t="s">
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="13">
+      <c r="D26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="11">
         <v>2</v>
       </c>
-      <c r="G26" s="17"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>61</v>
@@ -1440,14 +1386,11 @@
       <c r="E27" s="10">
         <v>3</v>
       </c>
-      <c r="F27" t="s">
-        <v>99</v>
-      </c>
-      <c r="G27" s="11"/>
+      <c r="G27" s="22"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>50</v>
@@ -1459,11 +1402,11 @@
       <c r="E28" s="10">
         <v>3</v>
       </c>
-      <c r="G28" s="11"/>
+      <c r="G28" s="22"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>58</v>
@@ -1477,70 +1420,77 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>29</v>
+      </c>
       <c r="B30" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>30</v>
+      </c>
       <c r="B31" s="10" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
-        <v>80</v>
-      </c>
-      <c r="G31" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>31</v>
+      </c>
       <c r="B32" s="10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="19"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>32</v>
+      </c>
       <c r="B33" s="10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>33</v>
+      </c>
       <c r="B34" s="10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" t="s">
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="G34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" t="s">
-        <v>101</v>
-      </c>
+      <c r="F35" s="18"/>
     </row>
     <row r="59" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J59" s="7"/>
@@ -1551,8 +1501,9 @@
       <sortCondition ref="E1:E57"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- fix bug add member - add workitem history
</commit_message>
<xml_diff>
--- a/Document/ProductBacklog.xlsx
+++ b/Document/ProductBacklog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
   <si>
     <t>create project</t>
   </si>
@@ -260,16 +260,10 @@
     <t>abort process</t>
   </si>
   <si>
-    <t>failed when email not invalid</t>
-  </si>
-  <si>
     <t>cannot create workitem when not be member</t>
   </si>
   <si>
     <t>attachtment</t>
-  </si>
-  <si>
-    <t>history</t>
   </si>
   <si>
     <t>my project</t>
@@ -360,7 +354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -384,15 +378,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -406,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -432,22 +417,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,7 +885,7 @@
   <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,11 +918,11 @@
       <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
@@ -954,7 +938,7 @@
       <c r="E2" s="10">
         <v>1</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="18"/>
       <c r="J2" s="19"/>
     </row>
@@ -988,7 +972,7 @@
       <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1110,11 +1094,9 @@
       <c r="E11" s="10">
         <v>1</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
@@ -1163,10 +1145,10 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>82</v>
       </c>
       <c r="H14" s="13" t="s">
         <v>24</v>
@@ -1202,9 +1184,6 @@
       <c r="E16" s="10">
         <v>1</v>
       </c>
-      <c r="F16" t="s">
-        <v>83</v>
-      </c>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1223,8 +1202,8 @@
       <c r="E17" s="4">
         <v>2</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="14"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
@@ -1386,7 +1365,7 @@
       <c r="E27" s="10">
         <v>3</v>
       </c>
-      <c r="G27" s="22"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
@@ -1402,7 +1381,7 @@
       <c r="E28" s="10">
         <v>3</v>
       </c>
-      <c r="G28" s="22"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
@@ -1485,7 +1464,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>

</xml_diff>